<commit_message>
Move all average updates to one task, add better rain gauge totals
</commit_message>
<xml_diff>
--- a/Device-Weather-Station-Firmware/MessageIDs.xlsx
+++ b/Device-Weather-Station-Firmware/MessageIDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/git/ProjectFishWorks-Node-Controller-Software/Device-Weather-Station/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\git\Device-WeatherStation\Device-Weather-Station-Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07B1F38-1D8F-E441-8CF8-86BD48B04E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFD101F-EA45-4BFF-81BC-4764189B37AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5800" yWindow="-21600" windowWidth="19160" windowHeight="21600" xr2:uid="{7AD2A4F0-F602-9249-9B83-84B49DEE1EFE}"/>
+    <workbookView xWindow="9210" yWindow="3360" windowWidth="19200" windowHeight="10310" xr2:uid="{7AD2A4F0-F602-9249-9B83-84B49DEE1EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Message ID</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>RTD Error Code</t>
+  </si>
+  <si>
+    <t>0x4001</t>
+  </si>
+  <si>
+    <t>Main Average Update Time</t>
   </si>
 </sst>
 </file>
@@ -521,18 +527,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FF347F-8880-5444-824F-08726C4B7A43}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,139 +546,147 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>